<commit_message>
added water highlighting and fish filtering
</commit_message>
<xml_diff>
--- a/assets/fishdata.xlsx
+++ b/assets/fishdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azure\Desktop\files\repos\FishFriend\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7E0117-E92B-4D69-89FF-3D7DA50F26EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B325C683-88F1-418F-A99E-6B4EEF7133AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E80F6E78-7DD6-4640-8733-4A29FA0C20F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E80F6E78-7DD6-4640-8733-4A29FA0C20F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="211">
   <si>
     <t>Name</t>
   </si>
@@ -291,9 +291,6 @@
     <t>112|139|168|225</t>
   </si>
   <si>
-    <t>Town River|Forest River|Waterfalls</t>
-  </si>
-  <si>
     <t>Walleye</t>
   </si>
   <si>
@@ -348,9 +345,6 @@
     <t>A common pond fish.</t>
   </si>
   <si>
-    <t>Mountain Lake|Secret Woods Pond|Sewer</t>
-  </si>
-  <si>
     <t>15 - 51</t>
   </si>
   <si>
@@ -615,9 +609,6 @@
     <t>Prefers temperature "edges" where cool and warm water meet.</t>
   </si>
   <si>
-    <t>6am - 11am|6pm - 2am</t>
-  </si>
-  <si>
     <t>20 - 41</t>
   </si>
   <si>
@@ -660,25 +651,13 @@
     <t>Halibut</t>
   </si>
   <si>
-    <t>6am - 11am|7pm - 2am</t>
-  </si>
-  <si>
     <t>Spring|Summer|Winter</t>
   </si>
   <si>
     <t>10 - 34</t>
   </si>
   <si>
-    <t>Town River|Forest River|Secret Woods Pond</t>
-  </si>
-  <si>
-    <t>Woodskip</t>
-  </si>
-  <si>
-    <t>A very sensitive fish that can only live in pools deep in the forest.</t>
-  </si>
-  <si>
-    <t>Secret Woods Pond</t>
+    <t>6am - 11am</t>
   </si>
 </sst>
 </file>
@@ -1041,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5974995B-DCE8-4A93-975D-7379999296AF}">
-  <dimension ref="A1:L418"/>
+  <dimension ref="A1:L417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,7 +1399,7 @@
         <v>87</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>38</v>
@@ -1443,34 +1422,34 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>83</v>
       </c>
       <c r="I11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>81</v>
@@ -1481,34 +1460,34 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>57</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>60</v>
@@ -1519,10 +1498,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>24</v>
@@ -1534,7 +1513,7 @@
         <v>26</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>57</v>
@@ -1546,10 +1525,10 @@
         <v>28</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>62</v>
@@ -1557,10 +1536,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>4</v>
@@ -1572,22 +1551,22 @@
         <v>6</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>214</v>
+        <v>55</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>62</v>
@@ -1595,10 +1574,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>35</v>
@@ -1610,7 +1589,7 @@
         <v>37</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>57</v>
@@ -1622,10 +1601,10 @@
         <v>28</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>31</v>
@@ -1633,10 +1612,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>24</v>
@@ -1654,13 +1633,13 @@
         <v>38</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>30</v>
@@ -1671,10 +1650,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>70</v>
@@ -1698,10 +1677,10 @@
         <v>28</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>42</v>
@@ -1709,7 +1688,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>44</v>
@@ -1730,16 +1709,16 @@
         <v>57</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>31</v>
@@ -1747,34 +1726,34 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>27</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>41</v>
@@ -1785,25 +1764,25 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>12</v>
@@ -1812,21 +1791,21 @@
         <v>28</v>
       </c>
       <c r="J20" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>46</v>
@@ -1844,16 +1823,16 @@
         <v>38</v>
       </c>
       <c r="H21" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>62</v>
@@ -1861,48 +1840,48 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J22" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>70</v>
@@ -1920,36 +1899,36 @@
         <v>38</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>9</v>
@@ -1958,27 +1937,27 @@
         <v>56</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>35</v>
@@ -1993,57 +1972,57 @@
         <v>9</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>61</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>62</v>
@@ -2051,10 +2030,10 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>4</v>
@@ -2081,7 +2060,7 @@
         <v>40</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>62</v>
@@ -2089,19 +2068,19 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>55</v>
@@ -2110,16 +2089,16 @@
         <v>38</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>31</v>
@@ -2127,10 +2106,10 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>70</v>
@@ -2157,7 +2136,7 @@
         <v>59</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="L29" s="3" t="s">
         <v>42</v>
@@ -2165,10 +2144,10 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>70</v>
@@ -2183,10 +2162,10 @@
         <v>9</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>28</v>
@@ -2203,10 +2182,10 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>46</v>
@@ -2218,7 +2197,7 @@
         <v>70</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>57</v>
@@ -2241,10 +2220,10 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>35</v>
@@ -2256,7 +2235,7 @@
         <v>37</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>38</v>
@@ -2268,10 +2247,10 @@
         <v>28</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>62</v>
@@ -2279,10 +2258,10 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>70</v>
@@ -2297,19 +2276,19 @@
         <v>9</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>62</v>
@@ -2317,10 +2296,10 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>47</v>
@@ -2329,22 +2308,22 @@
         <v>70</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>55</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>81</v>
@@ -2355,19 +2334,19 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>79</v>
@@ -2376,16 +2355,16 @@
         <v>57</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>62</v>
@@ -2393,79 +2372,53 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="K36" s="3" t="s">
         <v>61</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="L37" s="3"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
@@ -7027,18 +6980,6 @@
       <c r="I417" s="3"/>
       <c r="L417" s="3"/>
     </row>
-    <row r="418" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A418" s="3"/>
-      <c r="B418" s="3"/>
-      <c r="C418" s="3"/>
-      <c r="D418" s="3"/>
-      <c r="E418" s="3"/>
-      <c r="F418" s="3"/>
-      <c r="G418" s="3"/>
-      <c r="H418" s="3"/>
-      <c r="I418" s="3"/>
-      <c r="L418" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>